<commit_message>
added a few lines
</commit_message>
<xml_diff>
--- a/Rosetta_stone.xlsx
+++ b/Rosetta_stone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifergates/github/Misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D-o\Documents\Scripting\github-repos\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6EF0F4-B3AC-624D-9573-834CAF351BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E04818-20A7-4BF4-8095-0E536D5C9FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23740" windowHeight="14980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Rosetta Stone</t>
   </si>
@@ -99,6 +99,29 @@
   </si>
   <si>
     <t>Path = Path[0:-1]</t>
+  </si>
+  <si>
+    <t>file_handle = open('test.txt', 'r')
+file_contents = file_handle.read()
+file_handle.close()</t>
+  </si>
+  <si>
+    <t>cat file.txt</t>
+  </si>
+  <si>
+    <t>type file.txt</t>
+  </si>
+  <si>
+    <t>for /f %x in (test.txt) do echo %x</t>
+  </si>
+  <si>
+    <t>Get-Content .\test.txt | ForEach-Object {write-host $_}</t>
+  </si>
+  <si>
+    <t>file_handle = open('test.txt', 'r')
+file_contents = file_handle.readlines()
+for line in file_contents:
+    print(line)</t>
   </si>
 </sst>
 </file>
@@ -123,19 +146,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Courier"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Courier"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="3" tint="-0.249977111117893"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -145,6 +155,19 @@
       <sz val="11"/>
       <color theme="3" tint="-0.249977111117893"/>
       <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -233,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -241,20 +264,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -598,28 +627,28 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="30.5" customWidth="1"/>
-    <col min="4" max="4" width="39.1640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="38.5546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="D1" s="7"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -627,116 +656,128 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="9"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="D8" s="9"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -744,129 +785,129 @@
         <v>23</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="9"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" s="9"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="9"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="9"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="9"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="9"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="9"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="9"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="9"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="9"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="9"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="9"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="9"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="9"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="9"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="9"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -880,7 +921,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -892,7 +933,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>